<commit_message>
made changes to the excelfile
</commit_message>
<xml_diff>
--- a/excelfile.xlsx
+++ b/excelfile.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>How does an excel sheet appear in Git</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>bah</t>
+  </si>
+  <si>
+    <t>changes here</t>
   </si>
 </sst>
 </file>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,6 +549,11 @@
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>